<commit_message>
Exceli lugemine katse 2
</commit_message>
<xml_diff>
--- a/Küsimused.xlsx
+++ b/Küsimused.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\Ülikool_reloaded\3. Mehatroonika projekt\IT\vendingprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A37FA6C-45C1-4D4C-AE87-660EDF20F3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E38CC0-B1EB-489E-A55E-917AA908BA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{2944CBCF-6DFD-44E2-8215-CA75CA290995}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2944CBCF-6DFD-44E2-8215-CA75CA290995}"/>
   </bookViews>
   <sheets>
     <sheet name="Grupp_1" sheetId="1" r:id="rId1"/>
@@ -488,7 +488,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Valed vastused ka excelis
</commit_message>
<xml_diff>
--- a/Küsimused.xlsx
+++ b/Küsimused.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\Ülikool_reloaded\3. Mehatroonika projekt\IT\vendingprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E38CC0-B1EB-489E-A55E-917AA908BA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF191FD-2A3B-46DE-B8D4-C13D0463B294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2944CBCF-6DFD-44E2-8215-CA75CA290995}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2944CBCF-6DFD-44E2-8215-CA75CA290995}"/>
   </bookViews>
   <sheets>
     <sheet name="Grupp_1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Küssa</t>
   </si>
@@ -125,6 +125,69 @@
   </si>
   <si>
     <t>proov3</t>
+  </si>
+  <si>
+    <t>Valik1</t>
+  </si>
+  <si>
+    <t>Valik2</t>
+  </si>
+  <si>
+    <t>Vlaik3</t>
+  </si>
+  <si>
+    <t>uni</t>
+  </si>
+  <si>
+    <t>õlu</t>
+  </si>
+  <si>
+    <t>valik3</t>
+  </si>
+  <si>
+    <t>Luts</t>
+  </si>
+  <si>
+    <t>Köstrihärra</t>
+  </si>
+  <si>
+    <t>Toots</t>
+  </si>
+  <si>
+    <t>Silinder</t>
+  </si>
+  <si>
+    <t>Trapets</t>
+  </si>
+  <si>
+    <t>Võrdhaarne trapets</t>
+  </si>
+  <si>
+    <t>Gravitatsioonikiirendus</t>
+  </si>
+  <si>
+    <t>Kliirensikiirendus</t>
+  </si>
+  <si>
+    <t>Keskringjoone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puutuja </t>
+  </si>
+  <si>
+    <t>Keskristsirge</t>
+  </si>
+  <si>
+    <t>Maksim</t>
+  </si>
+  <si>
+    <t>Einstein</t>
+  </si>
+  <si>
+    <t>Galileo</t>
+  </si>
+  <si>
+    <t>Kiirendusvõistlus</t>
   </si>
 </sst>
 </file>
@@ -485,20 +548,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728BEA62-F630-4F6C-A633-F27681A3BC42}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="74.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,10 +569,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -517,18 +589,36 @@
         <v>8</v>
       </c>
       <c r="C2">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -541,20 +631,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76785A13-83EB-4155-886C-9E5565477D2B}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="102.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,59 +654,116 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
.hide() aitab asju ära peita
</commit_message>
<xml_diff>
--- a/Küsimused.xlsx
+++ b/Küsimused.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lootu\OneDrive\Desktop\Github\vendingprojekt-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\Ülikool_reloaded\3. Mehatroonika projekt\IT\vendingprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F8B719-47EF-4A3D-B3C6-CBB261B2616D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259A5D2C-F799-414C-9261-D701E1AFCEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="20868" windowHeight="12012" activeTab="2" xr2:uid="{2944CBCF-6DFD-44E2-8215-CA75CA290995}"/>
+    <workbookView xWindow="-105" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2944CBCF-6DFD-44E2-8215-CA75CA290995}"/>
   </bookViews>
   <sheets>
     <sheet name="Grupp_1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>Küssa</t>
   </si>
@@ -551,14 +551,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="74.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="74.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -598,7 +598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -615,7 +615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -630,20 +630,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76785A13-83EB-4155-886C-9E5565477D2B}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="102.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" customWidth="1"/>
-    <col min="4" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="102.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -683,7 +683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -703,7 +703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -723,7 +723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -743,7 +743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -770,20 +770,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33252635-A11D-41C3-8881-606A1B9AA576}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="96.6640625" customWidth="1"/>
+    <col min="1" max="1" width="96.7109375" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -791,10 +794,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -804,8 +816,11 @@
       <c r="C2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -815,8 +830,11 @@
       <c r="C3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -826,29 +844,41 @@
       <c r="C4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Küsimused enam ei kordu, pole raspi peal proovitud
</commit_message>
<xml_diff>
--- a/Küsimused.xlsx
+++ b/Küsimused.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livettu.sharepoint.com/sites/Tootmistehnika/Shared Documents/Mehhatroonika projekt/04_IT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\Ülikool_reloaded\3. Mehatroonika projekt\IT\vendingprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="251" documentId="13_ncr:1_{A8E375BE-246D-42EB-AE99-BC7BF0529220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BCBE0D0-FAC5-415A-8481-3430DD6F5FA8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEDCEA7-E078-4871-8710-479254AC6491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2944CBCF-6DFD-44E2-8215-CA75CA290995}"/>
+    <workbookView xWindow="-105" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2944CBCF-6DFD-44E2-8215-CA75CA290995}"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="4" r:id="rId1"/>
@@ -770,15 +770,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1238,7 +1234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728BEA62-F630-4F6C-A633-F27681A3BC42}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -1722,393 +1718,393 @@
     <col min="8" max="8" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" t="s">
         <v>70</v>
       </c>
-      <c r="F8" s="6">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>110</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" t="s">
         <v>112</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" t="s">
         <v>113</v>
       </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" t="s">
         <v>119</v>
       </c>
-      <c r="F10" s="6">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>164</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" t="s">
         <v>165</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" t="s">
         <v>166</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" t="s">
         <v>167</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" t="s">
         <v>168</v>
       </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="6">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>170</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" t="s">
         <v>172</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" t="s">
         <v>171</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" t="s">
         <v>173</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" t="s">
         <v>174</v>
       </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="6">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>175</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" t="s">
         <v>176</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" t="s">
         <v>177</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" t="s">
         <v>178</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" t="s">
         <v>179</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13">
         <v>1</v>
       </c>
-      <c r="G13" s="6">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>180</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" t="s">
         <v>184</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" t="s">
         <v>181</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" t="s">
         <v>182</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" t="s">
         <v>183</v>
       </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="H14" s="6">
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>195</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" t="s">
         <v>196</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" t="s">
         <v>197</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" t="s">
         <v>198</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" t="s">
         <v>199</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6">
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>2</v>
       </c>
     </row>
@@ -2121,7 +2117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33252635-A11D-41C3-8881-606A1B9AA576}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -2403,6 +2399,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A5508CC596D91468A4B201947B3B280" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14a927ece4f3ea2a91f30cf304bc7235">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="870dce62-94b7-4185-9b0a-7139e4ecfd19" xmlns:ns3="d36953de-bf6f-4d09-a956-94a114c2afc4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d7e2e7fca528be30e87c80d0fbe5901d" ns2:_="" ns3:_="">
     <xsd:import namespace="870dce62-94b7-4185-9b0a-7139e4ecfd19"/>
@@ -2597,15 +2602,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2618,6 +2614,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D4AF99-232C-48F0-A5C9-BB1B5A9492D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E8E05AB-1B47-4C51-8E09-465A5CFFA283}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2632,14 +2636,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D4AF99-232C-48F0-A5C9-BB1B5A9492D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
uued küssad ja pildid
</commit_message>
<xml_diff>
--- a/Küsimused.xlsx
+++ b/Küsimused.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\Ülikool_reloaded\3. Mehatroonika projekt\IT\vendingprojekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livettu.sharepoint.com/sites/Tootmistehnika/Shared Documents/Mehhatroonika projekt/04_IT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEDCEA7-E078-4871-8710-479254AC6491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080113DC-20E2-45C2-821F-035B6EEA8232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2944CBCF-6DFD-44E2-8215-CA75CA290995}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2944CBCF-6DFD-44E2-8215-CA75CA290995}"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="286">
+  <si>
+    <t>Kuidas seda Exceli faili kasutada‽</t>
+  </si>
   <si>
     <t>Käesolev fail sisaldab müügiautomaadis kuvatavaid küsimusi. Küsimused on vanusegruppide järgi jaotatud kolmele alalehele.</t>
   </si>
@@ -124,540 +127,6 @@
   </si>
   <si>
     <t>Ära kustuta tabelist ridu! Kustuta vaid rea sisu!</t>
-  </si>
-  <si>
-    <t>Küssa</t>
-  </si>
-  <si>
-    <t>Vastus</t>
-  </si>
-  <si>
-    <t>Valik1</t>
-  </si>
-  <si>
-    <t>Valik2</t>
-  </si>
-  <si>
-    <t>Valik3</t>
-  </si>
-  <si>
-    <t>Pilt</t>
-  </si>
-  <si>
-    <t>Vanusegrupp</t>
-  </si>
-  <si>
-    <t>Mis on elu mõte?</t>
-  </si>
-  <si>
-    <t>Ei tea</t>
-  </si>
-  <si>
-    <t>uni</t>
-  </si>
-  <si>
-    <t>õlu</t>
-  </si>
-  <si>
-    <t>Jukul on 4 ragulkat, õpetaja konfiskeerib neist 75%. Mitu ragulkat on Jukul alles?</t>
-  </si>
-  <si>
-    <t>Mis oli Kevades kandlemängiaja nimi?</t>
-  </si>
-  <si>
-    <t>Imelik</t>
-  </si>
-  <si>
-    <t>Luts</t>
-  </si>
-  <si>
-    <t>Köstrihärra</t>
-  </si>
-  <si>
-    <t>Toots</t>
-  </si>
-  <si>
-    <t>Nagu ruut on ristküliku alamliik, on ka romb mille alamliik?</t>
-  </si>
-  <si>
-    <t>Rööpkülik</t>
-  </si>
-  <si>
-    <t>Silinder</t>
-  </si>
-  <si>
-    <t>Trapets</t>
-  </si>
-  <si>
-    <t>Võrdhaarne trapets</t>
-  </si>
-  <si>
-    <t>Suunamuutusest tingitud kiirendus, mis on alati trajektoori kõveruskeskpunkti poole suunatud?</t>
-  </si>
-  <si>
-    <t>Kesktõmbekiirendus</t>
-  </si>
-  <si>
-    <t>Gravitatsioonikiirendus</t>
-  </si>
-  <si>
-    <t>Kliirensikiirendus</t>
-  </si>
-  <si>
-    <t>Kiirendusvõistlus</t>
-  </si>
-  <si>
-    <t>Täisnurkses kolmnurgas on kaatetitte ruutude summa võrdne mille ruuduga?</t>
-  </si>
-  <si>
-    <t>Hüpotenuusi</t>
-  </si>
-  <si>
-    <t>Keskringjoone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Puutuja </t>
-  </si>
-  <si>
-    <t>Keskristsirge</t>
-  </si>
-  <si>
-    <t>See inglasest teadjamees, kes on tuntud puuviljaga vastu pead saamise läbi, pani aluse klassikalisele mehaanikale.</t>
-  </si>
-  <si>
-    <t>Sir Isaac Newton</t>
-  </si>
-  <si>
-    <t>Sir Hiram Maxim</t>
-  </si>
-  <si>
-    <t>Albert Einstein</t>
-  </si>
-  <si>
-    <t>Galileo Galilei</t>
-  </si>
-  <si>
-    <t>Milline järgnevatest füüsikaseadustest, -printsiipidest või võrranditest on peamiselt seotud elektrotehnikaga?</t>
-  </si>
-  <si>
-    <t>Kirchoffi seadus</t>
-  </si>
-  <si>
-    <t>Langmuiri võrrand</t>
-  </si>
-  <si>
-    <t>Van der Waalsi jõud</t>
-  </si>
-  <si>
-    <t>Daltoni seadus</t>
-  </si>
-  <si>
-    <t>Mis on elekter?</t>
-  </si>
-  <si>
-    <t>Elektronide suunatud liikumine</t>
-  </si>
-  <si>
-    <t>Prootonite tavapäratu liikumine</t>
-  </si>
-  <si>
-    <t>Neutronite vaba liikumine</t>
-  </si>
-  <si>
-    <t>Mitte ükski nendest variantidest</t>
-  </si>
-  <si>
-    <t>Mis on e^x tuletis?</t>
-  </si>
-  <si>
-    <t>e^x</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>e^2x</t>
-  </si>
-  <si>
-    <t>e^e</t>
-  </si>
-  <si>
-    <t>Millega iseloomustatakse vedeliku voolamise laadi?</t>
-  </si>
-  <si>
-    <t>Reynoldsi arvuga</t>
-  </si>
-  <si>
-    <t>Boltzmani konstandiga</t>
-  </si>
-  <si>
-    <t>Rydbergi konstandiga</t>
-  </si>
-  <si>
-    <t>Hessi seadusega</t>
-  </si>
-  <si>
-    <t>1 moolses ainehulgas olevate aineosakeste hulka kirjeldab kelle nimeline arv?</t>
-  </si>
-  <si>
-    <t>Avogadro</t>
-  </si>
-  <si>
-    <t>Kirchoffi</t>
-  </si>
-  <si>
-    <t>Wieni</t>
-  </si>
-  <si>
-    <t>Henry</t>
-  </si>
-  <si>
-    <t>Kodutarbija maksab aktiivvõimsuse eest. Millise võimsuse eest peavad maksma vaid tööstuslikud tarbijad?</t>
-  </si>
-  <si>
-    <t>Reaktiivvõimsus</t>
-  </si>
-  <si>
-    <t>Aktiivvõimsus</t>
-  </si>
-  <si>
-    <t>Pöördvõimsus</t>
-  </si>
-  <si>
-    <t>Tootmisvõimsus</t>
-  </si>
-  <si>
-    <t>Võrrand, mis seob otsitavaid funktsioone, nende tuletisi ja argumente on tuntud kui</t>
-  </si>
-  <si>
-    <t>Diferentsiaalvõrrand</t>
-  </si>
-  <si>
-    <t>Eksponentsiaalvõrrand</t>
-  </si>
-  <si>
-    <t>Logaritmvõrrand</t>
-  </si>
-  <si>
-    <t>Diofantiline võrrand</t>
-  </si>
-  <si>
-    <t>Üks olulisemaid füüsikaseaduseid, mis väidab, et isoleeritud süsteemi energia on ajas muutumatu suurus.</t>
-  </si>
-  <si>
-    <t>Energia jäävuse seadus</t>
-  </si>
-  <si>
-    <t>Plancki kiirgusseadus</t>
-  </si>
-  <si>
-    <t>Gravitatsiooniseadus</t>
-  </si>
-  <si>
-    <t>Inertsiseadus</t>
-  </si>
-  <si>
-    <t>Joondefekt</t>
-  </si>
-  <si>
-    <t>Punkdefekt</t>
-  </si>
-  <si>
-    <t>Pinnadefekt</t>
-  </si>
-  <si>
-    <t>Ruumidefekt</t>
-  </si>
-  <si>
-    <t>Tõmbel ristsuunas ahenemise suhe telgsuunas pikenemisele on tuntud</t>
-  </si>
-  <si>
-    <t>Poissoni tegurina</t>
-  </si>
-  <si>
-    <t>joonpaisumistegurina</t>
-  </si>
-  <si>
-    <t>pingeintensiivsustegurina</t>
-  </si>
-  <si>
-    <t>hõõrdetegurina</t>
-  </si>
-  <si>
-    <t>Milline järgnevatest ühikutest ei kuulu SI ühikute süsteemi?</t>
-  </si>
-  <si>
-    <t>cd (kandela)</t>
-  </si>
-  <si>
-    <t>K (Kelvin)</t>
-  </si>
-  <si>
-    <t>A (amper)</t>
-  </si>
-  <si>
-    <t>atm (atmosfäär)</t>
-  </si>
-  <si>
-    <t>Mida mõõdetakse radiaanides?</t>
-  </si>
-  <si>
-    <t>Nurka</t>
-  </si>
-  <si>
-    <t>Ruuminurka</t>
-  </si>
-  <si>
-    <t>Nurkkiirust</t>
-  </si>
-  <si>
-    <t>Pöördenurka</t>
-  </si>
-  <si>
-    <t>Mida mõõdetakse sterradiaanides?</t>
-  </si>
-  <si>
-    <t>Mida mõõdetakse ebaharilike mõõtühikutega jalg, toll, küünar, vaks ja süld?</t>
-  </si>
-  <si>
-    <t>Pikkust</t>
-  </si>
-  <si>
-    <t>Massi</t>
-  </si>
-  <si>
-    <t>Ruumala</t>
-  </si>
-  <si>
-    <t>Temperatuuri</t>
-  </si>
-  <si>
-    <t>Millisels olekus täidab aine ühtlaselt kogu tema käsutusse antud ruumala?</t>
-  </si>
-  <si>
-    <t>Gaasilises olekus</t>
-  </si>
-  <si>
-    <t>Tahkes olekus</t>
-  </si>
-  <si>
-    <t>Vedelas olekus</t>
-  </si>
-  <si>
-    <t>Jäätunud olekus</t>
-  </si>
-  <si>
-    <t>Kui kodusea süda lööb keskmiselt 4200 korda tunnis, siis mitu korda lööb see keskmiselt minutis?</t>
-  </si>
-  <si>
-    <t>Kirjapilt |-x| annab mõista, et …</t>
-  </si>
-  <si>
-    <t>muutujat x tuleb ignoreerida</t>
-  </si>
-  <si>
-    <t>viidatakse ruutjuurele</t>
-  </si>
-  <si>
-    <t>viidatakse absoluutväärtusele</t>
-  </si>
-  <si>
-    <t>muutuja x tuleb kahekordistada</t>
-  </si>
-  <si>
-    <t>Teatrisaalis on 2000 istekohta. 85% neist asub parteris, ülejäänud rõdul. Mitu kohta on rõdul?</t>
-  </si>
-  <si>
-    <t>Milline järgnevatest arvudes jaguneb 9-ga?</t>
-  </si>
-  <si>
-    <t>Iga võrdkülgne kolmnurk on ühtlasi ka …</t>
-  </si>
-  <si>
-    <t>Võrdhaarne</t>
-  </si>
-  <si>
-    <t>Täisnurkne</t>
-  </si>
-  <si>
-    <t>Nürinurkne</t>
-  </si>
-  <si>
-    <t>Parelleelne</t>
-  </si>
-  <si>
-    <t>Mis on inimese kõige suurem elund?</t>
-  </si>
-  <si>
-    <t>Nahk</t>
-  </si>
-  <si>
-    <t>Maks</t>
-  </si>
-  <si>
-    <t>Kopsud</t>
-  </si>
-  <si>
-    <t>Aju</t>
-  </si>
-  <si>
-    <t>Milline järgnevatest ei ole elu tunnus?</t>
-  </si>
-  <si>
-    <t>Toittumine</t>
-  </si>
-  <si>
-    <t>Paljunemine</t>
-  </si>
-  <si>
-    <t>Rakkudest koosnemine</t>
-  </si>
-  <si>
-    <t>Liikumine</t>
-  </si>
-  <si>
-    <t>Joon, mis jagab Maa põhja ja lõunapoolkeraks, on …</t>
-  </si>
-  <si>
-    <t>ekvaator</t>
-  </si>
-  <si>
-    <t>meridiaan</t>
-  </si>
-  <si>
-    <t>pöörijoon</t>
-  </si>
-  <si>
-    <t>pikkusjoon</t>
-  </si>
-  <si>
-    <t>Ekvaatoriga on paralleelsed …</t>
-  </si>
-  <si>
-    <t>laiusjooned</t>
-  </si>
-  <si>
-    <t>pikkusjooned</t>
-  </si>
-  <si>
-    <t>meridiaanid</t>
-  </si>
-  <si>
-    <t>samakõrgusjooned</t>
-  </si>
-  <si>
-    <t>Maapinna samal kõrgusel asuvaid lõikeid kujutavad kaartidel …</t>
-  </si>
-  <si>
-    <t>isohüpsid</t>
-  </si>
-  <si>
-    <t>hüdroisohüpsid</t>
-  </si>
-  <si>
-    <t>isotermid</t>
-  </si>
-  <si>
-    <t>isobaarid</t>
-  </si>
-  <si>
-    <t>Kui kaardi mõõtkava on 1:50000, siis üks sentimeeter kaardil on võrdne … meetriga looduses.</t>
-  </si>
-  <si>
-    <t>Asimuut kirjeldab suunda  … suhtes.</t>
-  </si>
-  <si>
-    <t>geograafilise põhja</t>
-  </si>
-  <si>
-    <t>magneetilise põhja</t>
-  </si>
-  <si>
-    <t>Põhjanaela</t>
-  </si>
-  <si>
-    <t>kartograafilise põhja</t>
-  </si>
-  <si>
-    <t>Mida on kujutatud joonisel A?</t>
-  </si>
-  <si>
-    <t>Laminaarset voolamist</t>
-  </si>
-  <si>
-    <t>Turbulentset voolamist</t>
-  </si>
-  <si>
-    <t>Potentsiaalset voolamist</t>
-  </si>
-  <si>
-    <t>Hõõrdumiseta voolamist</t>
-  </si>
-  <si>
-    <t>Milline järgnevatest ei ole vesiniku isotoop?</t>
-  </si>
-  <si>
-    <t>Deuteerium</t>
-  </si>
-  <si>
-    <t>Triitium</t>
-  </si>
-  <si>
-    <t>Prootium</t>
-  </si>
-  <si>
-    <t>Luteetium</t>
-  </si>
-  <si>
-    <t>Mille vari langeb Kuule kuuvarjutuse ajal?</t>
-  </si>
-  <si>
-    <t>Maa</t>
-  </si>
-  <si>
-    <t>Kuu</t>
-  </si>
-  <si>
-    <t>Asteroidide</t>
-  </si>
-  <si>
-    <t>Marsi</t>
-  </si>
-  <si>
-    <t>Maa on …</t>
-  </si>
-  <si>
-    <t>Ümmargune</t>
-  </si>
-  <si>
-    <t>Lapik</t>
-  </si>
-  <si>
-    <t>Sõõriku kujuline</t>
-  </si>
-  <si>
-    <t>Hüperboloid</t>
-  </si>
-  <si>
-    <t>Milline pildil toodud geomeetriline pind oli Vennaskonna esitatud laulus Insener Garini üks lemmikuid?</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Kristallvõredes esineb mitmeid defekte. Millist defektiliiki tuntakse ka kui disloaktsiooni?</t>
-  </si>
-  <si>
-    <t>Sisestus</t>
   </si>
   <si>
     <r>
@@ -710,14 +179,788 @@
     <t>Teiste vastuste tulbad võib tühjaks jätta.</t>
   </si>
   <si>
-    <t>Kuidas seda Exceli faili kasutada‽</t>
+    <t>Küssa</t>
+  </si>
+  <si>
+    <t>Vastus</t>
+  </si>
+  <si>
+    <t>Valik1</t>
+  </si>
+  <si>
+    <t>Valik2</t>
+  </si>
+  <si>
+    <t>Valik3</t>
+  </si>
+  <si>
+    <t>Pilt</t>
+  </si>
+  <si>
+    <t>Sisestus</t>
+  </si>
+  <si>
+    <t>Vanusegrupp</t>
+  </si>
+  <si>
+    <t>Mis on elu mõte?</t>
+  </si>
+  <si>
+    <t>Ei tea</t>
+  </si>
+  <si>
+    <t>uni</t>
+  </si>
+  <si>
+    <t>õlu</t>
+  </si>
+  <si>
+    <t>Jukul on 4 ragulkat, õpetaja konfiskeerib neist 75%. Mitu ragulkat on Jukul alles?</t>
+  </si>
+  <si>
+    <t>Mida mõõdetakse ebaharilike mõõtühikutega jalg, toll, küünar, vaks ja süld?</t>
+  </si>
+  <si>
+    <t>Pikkust</t>
+  </si>
+  <si>
+    <t>Massi</t>
+  </si>
+  <si>
+    <t>Ruumala</t>
+  </si>
+  <si>
+    <t>Temperatuuri</t>
+  </si>
+  <si>
+    <t>Millises olekus täidab aine ühtlaselt kogu tema käsutusse antud ruumala?</t>
+  </si>
+  <si>
+    <t>Gaasilises olekus</t>
+  </si>
+  <si>
+    <t>Tahkes olekus</t>
+  </si>
+  <si>
+    <t>Vedelas olekus</t>
+  </si>
+  <si>
+    <t>Jäätunud olekus</t>
+  </si>
+  <si>
+    <t>Kui kodusea süda lööb keskmiselt 4200 korda tunnis, siis mitu korda lööb see keskmiselt minutis?</t>
+  </si>
+  <si>
+    <t>Kirjapilt |-x| annab mõista, et …</t>
+  </si>
+  <si>
+    <t>viidatakse absoluutväärtusele</t>
+  </si>
+  <si>
+    <t>viidatakse ruutjuurele</t>
+  </si>
+  <si>
+    <t>muutujat x tuleb ignoreerida</t>
+  </si>
+  <si>
+    <t>muutuja x tuleb kahekordistada</t>
+  </si>
+  <si>
+    <t>Teatrisaalis on 2000 istekohta. 85% neist asub parteris, ülejäänud rõdul. Mitu kohta on rõdul?</t>
+  </si>
+  <si>
+    <t>Milline järgnevatest arvudes jaguneb 9-ga?</t>
+  </si>
+  <si>
+    <t>Iga võrdkülgne kolmnurk on ühtlasi ka …</t>
+  </si>
+  <si>
+    <t>Teravnurkne</t>
+  </si>
+  <si>
+    <t>Täisnurkne</t>
+  </si>
+  <si>
+    <t>Nürinurkne</t>
+  </si>
+  <si>
+    <t>Parelleelne</t>
+  </si>
+  <si>
+    <t>Mis on inimese kõige suurem elund?</t>
+  </si>
+  <si>
+    <t>Nahk</t>
+  </si>
+  <si>
+    <t>Maks</t>
+  </si>
+  <si>
+    <t>Kopsud</t>
+  </si>
+  <si>
+    <t>Aju</t>
+  </si>
+  <si>
+    <t>Milline järgnevatest ei ole elu tunnus?</t>
+  </si>
+  <si>
+    <t>Liikumine</t>
+  </si>
+  <si>
+    <t>Toitumine</t>
+  </si>
+  <si>
+    <t>Paljunemine</t>
+  </si>
+  <si>
+    <t>Rakkudest koosnemine</t>
+  </si>
+  <si>
+    <t>Joon, mis jagab Maa põhja ja lõunapoolkeraks, on …</t>
+  </si>
+  <si>
+    <t>ekvaator</t>
+  </si>
+  <si>
+    <t>meridiaan</t>
+  </si>
+  <si>
+    <t>pöörijoon</t>
+  </si>
+  <si>
+    <t>pikkusjoon</t>
+  </si>
+  <si>
+    <t>Ekvaatoriga on paralleelsed …</t>
+  </si>
+  <si>
+    <t>laiusjooned</t>
+  </si>
+  <si>
+    <t>pikkusjooned</t>
+  </si>
+  <si>
+    <t>meridiaanid</t>
+  </si>
+  <si>
+    <t>samakõrgusjooned</t>
+  </si>
+  <si>
+    <t>Kui kaardi mõõtkava on 1:50000, siis üks sentimeeter kaardil on võrdne … meetriga looduses.</t>
+  </si>
+  <si>
+    <t>Mille vari langeb Kuule kuuvarjutuse ajal?</t>
+  </si>
+  <si>
+    <t>Maa</t>
+  </si>
+  <si>
+    <t>Kuu</t>
+  </si>
+  <si>
+    <t>Marsi</t>
+  </si>
+  <si>
+    <t>Asteroidide</t>
+  </si>
+  <si>
+    <t>Maa on …</t>
+  </si>
+  <si>
+    <t>Ümmargune</t>
+  </si>
+  <si>
+    <t>Lapik</t>
+  </si>
+  <si>
+    <t>Sõõriku kujuline</t>
+  </si>
+  <si>
+    <t>Hüperboloid</t>
+  </si>
+  <si>
+    <t>Vaal on ...</t>
+  </si>
+  <si>
+    <t>Imetaja</t>
+  </si>
+  <si>
+    <t>Lind</t>
+  </si>
+  <si>
+    <t>Kala</t>
+  </si>
+  <si>
+    <t>Kahepaikne</t>
+  </si>
+  <si>
+    <t>Jukul on 6 õuna, ta annab pooled neist Marile. Mitu õuna jäi Jukule?</t>
+  </si>
+  <si>
+    <t>Miks on saunas kõrgemal istudes õhk kuumem kui põranda lähedal olles?</t>
+  </si>
+  <si>
+    <t>Kuumus tõuseb üles</t>
+  </si>
+  <si>
+    <t>Seal on niiskem</t>
+  </si>
+  <si>
+    <t>Põrandal on sama kuum</t>
+  </si>
+  <si>
+    <t>Külm ei saa kuumaga läbi</t>
+  </si>
+  <si>
+    <t>Arvuta: (4 x 4 + 44) : 4 + 4 =</t>
+  </si>
+  <si>
+    <t>Mitu nelinurka on joonisel?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kahte liiki klotsidest ehitati joonisel olev risttahukas. Väiksemad klotsid olid kõik kuubid servapikkusega 1 dm. Leia risttahuka pikkus. </t>
+  </si>
+  <si>
+    <t>15 dm</t>
+  </si>
+  <si>
+    <t>17 dm</t>
+  </si>
+  <si>
+    <t>13 dm</t>
+  </si>
+  <si>
+    <t>16 dm</t>
+  </si>
+  <si>
+    <t>Mis oli Kevades kandlemängiaja nimi?</t>
+  </si>
+  <si>
+    <t>Imelik</t>
+  </si>
+  <si>
+    <t>Luts</t>
+  </si>
+  <si>
+    <t>Köstrihärra</t>
+  </si>
+  <si>
+    <t>Toots</t>
+  </si>
+  <si>
+    <t>Nagu ruut on ristküliku alamliik, on ka romb mille alamliik?</t>
+  </si>
+  <si>
+    <t>Rööpkülik</t>
+  </si>
+  <si>
+    <t>Silinder</t>
+  </si>
+  <si>
+    <t>Trapets</t>
+  </si>
+  <si>
+    <t>Võrdhaarne trapets</t>
+  </si>
+  <si>
+    <t>Suunamuutusest tingitud kiirendus, mis on alati trajektoori kõveruskeskpunkti poole suunatud?</t>
+  </si>
+  <si>
+    <t>Kesktõmbekiirendus</t>
+  </si>
+  <si>
+    <t>Gravitatsioonikiirendus</t>
+  </si>
+  <si>
+    <t>Kliirensikiirendus</t>
+  </si>
+  <si>
+    <t>Kiirendusvõistlus</t>
+  </si>
+  <si>
+    <t>Täisnurkses kolmnurgas on kaatetite ruutude summa võrdne mille ruuduga?</t>
+  </si>
+  <si>
+    <t>Hüpotenuusi</t>
+  </si>
+  <si>
+    <t>Keskringjoone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puutuja </t>
+  </si>
+  <si>
+    <t>Keskristsirge</t>
+  </si>
+  <si>
+    <t>See inglasest teadjamees, kes on tuntud puuviljaga vastu pead saamise läbi, pani aluse klassikalisele mehaanikale.</t>
+  </si>
+  <si>
+    <t>Sir Isaac Newton</t>
+  </si>
+  <si>
+    <t>Sir Hiram Maxim</t>
+  </si>
+  <si>
+    <t>Albert Einstein</t>
+  </si>
+  <si>
+    <t>Galileo Galilei</t>
+  </si>
+  <si>
+    <t>Milline järgnevatest füüsikaseadustest, -printsiipidest või võrranditest on peamiselt seotud elektrotehnikaga?</t>
+  </si>
+  <si>
+    <t>Kirchoffi seadus</t>
+  </si>
+  <si>
+    <t>Langmuiri võrrand</t>
+  </si>
+  <si>
+    <t>Van der Waalsi jõud</t>
+  </si>
+  <si>
+    <t>Daltoni seadus</t>
+  </si>
+  <si>
+    <t>Mis on elekter?</t>
+  </si>
+  <si>
+    <t>Elektronide suunatud liikumine</t>
+  </si>
+  <si>
+    <t>Prootonite tavapäratu liikumine</t>
+  </si>
+  <si>
+    <t>Neutronite vaba liikumine</t>
+  </si>
+  <si>
+    <t>Mitte ükski nendest variantidest</t>
+  </si>
+  <si>
+    <t>Milline järgnevatest ühikutest ei kuulu SI ühikute süsteemi?</t>
+  </si>
+  <si>
+    <t>atm (atmosfäär)</t>
+  </si>
+  <si>
+    <t>cd (kandela)</t>
+  </si>
+  <si>
+    <t>K (Kelvin)</t>
+  </si>
+  <si>
+    <t>A (amper)</t>
+  </si>
+  <si>
+    <t>Mida mõõdetakse radiaanides?</t>
+  </si>
+  <si>
+    <t>Nurka</t>
+  </si>
+  <si>
+    <t>Ruuminurka</t>
+  </si>
+  <si>
+    <t>Nurkkiirust</t>
+  </si>
+  <si>
+    <t>Pöördenurka</t>
+  </si>
+  <si>
+    <t>Maapinna samal kõrgusel asuvaid lõikeid kujutavad kaartidel …</t>
+  </si>
+  <si>
+    <t>isohüpsid</t>
+  </si>
+  <si>
+    <t>hüdroisohüpsid</t>
+  </si>
+  <si>
+    <t>isotermid</t>
+  </si>
+  <si>
+    <t>isobaarid</t>
+  </si>
+  <si>
+    <t>Asimuut kirjeldab suunda  … suhtes.</t>
+  </si>
+  <si>
+    <t>magneetilise põhja</t>
+  </si>
+  <si>
+    <t>geograafilise põhja</t>
+  </si>
+  <si>
+    <t>Põhjanaela</t>
+  </si>
+  <si>
+    <t>kartograafilise põhja</t>
+  </si>
+  <si>
+    <t>Mida on kujutatud joonisel A?</t>
+  </si>
+  <si>
+    <t>Laminaarset voolamist</t>
+  </si>
+  <si>
+    <t>Turbulentset voolamist</t>
+  </si>
+  <si>
+    <t>Potentsiaalset voolamist</t>
+  </si>
+  <si>
+    <t>Hõõrdumiseta voolamist</t>
+  </si>
+  <si>
+    <t>Milline järgnevatest ei ole vesiniku isotoop?</t>
+  </si>
+  <si>
+    <t>Luteetium</t>
+  </si>
+  <si>
+    <t>Deuteerium</t>
+  </si>
+  <si>
+    <t>Triitium</t>
+  </si>
+  <si>
+    <t>Prootium</t>
+  </si>
+  <si>
+    <t>Milline pildil toodud geomeetriline pind oli Vennaskonna esitatud laulus Insener Garini üks lemmikuid?</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Millise laenguga kehad tõmbuvad?</t>
+  </si>
+  <si>
+    <t>Erinimelise</t>
+  </si>
+  <si>
+    <t>Samanimelise</t>
+  </si>
+  <si>
+    <t>Vastunimelise</t>
+  </si>
+  <si>
+    <t>Koosnimeline</t>
+  </si>
+  <si>
+    <t>Mida hüüdis Archimedes, kui ta avastas et veega saab keha ruumala mõõta?</t>
+  </si>
+  <si>
+    <t>Eureka</t>
+  </si>
+  <si>
+    <t>Juhhei</t>
+  </si>
+  <si>
+    <t>OMG</t>
+  </si>
+  <si>
+    <t>Yippee Ki Yay</t>
+  </si>
+  <si>
+    <t>Kes on pildil?</t>
+  </si>
+  <si>
+    <t>Robert Oppenheimer</t>
+  </si>
+  <si>
+    <t>Steven Hawking</t>
+  </si>
+  <si>
+    <t>Archimedes</t>
+  </si>
+  <si>
+    <t>Mis tingimusel avaneb funktsioon y=ax²+bx+c üles</t>
+  </si>
+  <si>
+    <t>a&gt;0</t>
+  </si>
+  <si>
+    <t>a&lt;0</t>
+  </si>
+  <si>
+    <t>a=0</t>
+  </si>
+  <si>
+    <t>b&gt;0</t>
+  </si>
+  <si>
+    <t>Kas leidub kolmnurk nurkade suurustega  A°, B° ja 60°, mille korral A° – B° = 60°?</t>
+  </si>
+  <si>
+    <t>Jah</t>
+  </si>
+  <si>
+    <t>Ei</t>
+  </si>
+  <si>
+    <t>Võib olla</t>
+  </si>
+  <si>
+    <t>Järgmine küsimus</t>
+  </si>
+  <si>
+    <t>Kahe täisarvu summa on 1 ja nende korrutis on −6. Leia nende arvude suurim võimalik vahe.</t>
+  </si>
+  <si>
+    <t>Õppeveerandi jooksul tuli teha 5 kontrolltesti. Iga testi eest võis saada kuni 100 punkti. Jüri nelja testi keskmine tulemus oli 75 punkti. Mitu punkti võib maksimaalselt olla tema viie testi keskmine tulemus?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ühesugustele kujunditele vastavad ühesugused arvud. Mitme võrra on ruudule vastav arv suurem kolmnurgale vastavast arvust? </t>
+  </si>
+  <si>
+    <t>Joonisel on kolm ühise keskpunktiga ringi ning suurima ringi neli diameetrit. Mitu protsenti suurimast ringist on tumedamaks värvitud?</t>
+  </si>
+  <si>
+    <t>Mis on e^x tuletis?</t>
+  </si>
+  <si>
+    <t>e^x</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>e^2x</t>
+  </si>
+  <si>
+    <t>e^e</t>
+  </si>
+  <si>
+    <t>Millega iseloomustatakse vedeliku voolamise laadi?</t>
+  </si>
+  <si>
+    <t>Reynoldsi arvuga</t>
+  </si>
+  <si>
+    <t>Boltzmani konstandiga</t>
+  </si>
+  <si>
+    <t>Rydbergi konstandiga</t>
+  </si>
+  <si>
+    <t>Hessi seadusega</t>
+  </si>
+  <si>
+    <t>1 moolses ainehulgas olevate aineosakeste hulka kirjeldab kelle nimeline arv?</t>
+  </si>
+  <si>
+    <t>Avogadro</t>
+  </si>
+  <si>
+    <t>Kirchoffi</t>
+  </si>
+  <si>
+    <t>Wieni</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Kodutarbija maksab aktiivvõimsuse eest. Millise võimsuse eest peavad maksma vaid tööstuslikud tarbijad?</t>
+  </si>
+  <si>
+    <t>Reaktiivvõimsus</t>
+  </si>
+  <si>
+    <t>Aktiivvõimsus</t>
+  </si>
+  <si>
+    <t>Pöördvõimsus</t>
+  </si>
+  <si>
+    <t>Tootmisvõimsus</t>
+  </si>
+  <si>
+    <t>Võrrand, mis seob otsitavaid funktsioone, nende tuletisi ja argumente on tuntud kui</t>
+  </si>
+  <si>
+    <t>Diferentsiaalvõrrand</t>
+  </si>
+  <si>
+    <t>Eksponentsiaalvõrrand</t>
+  </si>
+  <si>
+    <t>Logaritmvõrrand</t>
+  </si>
+  <si>
+    <t>Diofantiline võrrand</t>
+  </si>
+  <si>
+    <t>Üks olulisemaid füüsikaseaduseid, mis väidab, et isoleeritud süsteemi energia on ajas muutumatu suurus.</t>
+  </si>
+  <si>
+    <t>Energia jäävuse seadus</t>
+  </si>
+  <si>
+    <t>Plancki kiirgusseadus</t>
+  </si>
+  <si>
+    <t>Gravitatsiooniseadus</t>
+  </si>
+  <si>
+    <t>Inertsiseadus</t>
+  </si>
+  <si>
+    <t>Kristallvõredes esineb mitmeid defekte. Millist defektiliiki tuntakse ka kui disloaktsiooni?</t>
+  </si>
+  <si>
+    <t>Joondefekt</t>
+  </si>
+  <si>
+    <t>Punkdefekt</t>
+  </si>
+  <si>
+    <t>Pinnadefekt</t>
+  </si>
+  <si>
+    <t>Ruumidefekt</t>
+  </si>
+  <si>
+    <t>Tõmbel ristsuunas ahenemise suhe telgsuunas pikenemisele on tuntud</t>
+  </si>
+  <si>
+    <t>Poissoni tegurina</t>
+  </si>
+  <si>
+    <t>joonpaisumistegurina</t>
+  </si>
+  <si>
+    <t>pingeintensiivsustegurina</t>
+  </si>
+  <si>
+    <t>hõõrdetegurina</t>
+  </si>
+  <si>
+    <t>Mida mõõdetakse sterradiaanides?</t>
+  </si>
+  <si>
+    <t>Mida tähistab number materjali tähises S235</t>
+  </si>
+  <si>
+    <t>Voolepiir</t>
+  </si>
+  <si>
+    <t>Kõvadus</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Maksimaalne tugevus</t>
+  </si>
+  <si>
+    <t>See imeraamat aitab inseneri igas hetkes...</t>
+  </si>
+  <si>
+    <t>Mehaanikainseneri käsiraamat</t>
+  </si>
+  <si>
+    <t>Piibel</t>
+  </si>
+  <si>
+    <t>Tõde ja õigus</t>
+  </si>
+  <si>
+    <t>Aabits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nelinurga ABCD küljel AB asub punkt E. Teada on, et AD = DC = CB = DE ning nurk DAB on suurusega 70° ja nurk ADC on suurusega 100°. Leia nurga CBA suurus.  </t>
+  </si>
+  <si>
+    <t>50°</t>
+  </si>
+  <si>
+    <t>80°</t>
+  </si>
+  <si>
+    <t>40°</t>
+  </si>
+  <si>
+    <t>60°</t>
+  </si>
+  <si>
+    <t>Mis on Lõuna-Korea suurima tehnoloogiaettevõtte nimi?</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Huawei</t>
+  </si>
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>Mis aastal leiutas toote WD40 keemik Norm Larsen?</t>
+  </si>
+  <si>
+    <t>1930. aastal anti Albert Einsteinile ja kolleegile välja USA patent 1781541. Milleks see mõeldud oli?</t>
+  </si>
+  <si>
+    <t>Külmik</t>
+  </si>
+  <si>
+    <t>Mikrolaineahi</t>
+  </si>
+  <si>
+    <t>Külmsuitsukapp</t>
+  </si>
+  <si>
+    <t>Pesumasin</t>
+  </si>
+  <si>
+    <t>Kes leiutas esimest lambipirni?</t>
+  </si>
+  <si>
+    <t>Humphry Davy</t>
+  </si>
+  <si>
+    <t>Thomas Edison</t>
+  </si>
+  <si>
+    <t>Nikola Tesla</t>
+  </si>
+  <si>
+    <t>Mis noot on punases ringis?</t>
+  </si>
+  <si>
+    <t>Fa</t>
+  </si>
+  <si>
+    <t>Mi</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>La</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -749,6 +992,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -770,11 +1019,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1081,7 +1340,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1092,136 +1351,136 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>204</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>202</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>203</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1232,16 +1491,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728BEA62-F630-4F6C-A633-F27681A3BC42}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="87.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" customWidth="1"/>
@@ -1252,45 +1511,45 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>201</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
+      <c r="D2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1304,18 +1563,18 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
+        <v>39</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>4</v>
       </c>
       <c r="F3">
@@ -1330,19 +1589,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" t="s">
-        <v>125</v>
+        <v>40</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1356,19 +1615,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" t="s">
-        <v>130</v>
+        <v>45</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1382,18 +1641,18 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="B6" s="6">
         <v>70</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>80</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>60</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>75</v>
       </c>
       <c r="F6">
@@ -1408,19 +1667,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" t="s">
-        <v>136</v>
+        <v>51</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1434,18 +1693,18 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8">
+        <v>56</v>
+      </c>
+      <c r="B8" s="6">
         <v>300</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>85</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>200</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>250</v>
       </c>
       <c r="F8">
@@ -1460,18 +1719,18 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9">
+        <v>57</v>
+      </c>
+      <c r="B9" s="6">
         <v>4374</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>4474</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>8735</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>2857</v>
       </c>
       <c r="F9">
@@ -1486,19 +1745,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" t="s">
-        <v>141</v>
-      </c>
-      <c r="D10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E10" t="s">
-        <v>143</v>
+        <v>58</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1512,19 +1771,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B11" t="s">
-        <v>145</v>
-      </c>
-      <c r="C11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D11" t="s">
-        <v>147</v>
-      </c>
-      <c r="E11" t="s">
-        <v>148</v>
+        <v>63</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1538,19 +1797,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" t="s">
-        <v>151</v>
-      </c>
-      <c r="E12" t="s">
-        <v>152</v>
+        <v>68</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1564,19 +1823,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" t="s">
-        <v>155</v>
-      </c>
-      <c r="C13" t="s">
-        <v>156</v>
-      </c>
-      <c r="D13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E13" t="s">
-        <v>158</v>
+        <v>73</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1590,19 +1849,19 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" t="s">
-        <v>160</v>
-      </c>
-      <c r="C14" t="s">
-        <v>161</v>
-      </c>
-      <c r="D14" t="s">
-        <v>162</v>
-      </c>
-      <c r="E14" t="s">
-        <v>163</v>
+        <v>78</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1616,18 +1875,18 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>169</v>
-      </c>
-      <c r="B15">
+        <v>83</v>
+      </c>
+      <c r="B15" s="6">
         <v>500</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>1000</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="6">
         <v>50</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="6">
         <v>100</v>
       </c>
       <c r="F15">
@@ -1642,19 +1901,19 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>185</v>
-      </c>
-      <c r="B16" t="s">
-        <v>186</v>
-      </c>
-      <c r="C16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D16" t="s">
-        <v>189</v>
-      </c>
-      <c r="E16" t="s">
-        <v>188</v>
+        <v>84</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1668,19 +1927,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>190</v>
-      </c>
-      <c r="B17" t="s">
-        <v>191</v>
-      </c>
-      <c r="C17" t="s">
-        <v>192</v>
-      </c>
-      <c r="D17" t="s">
-        <v>193</v>
-      </c>
-      <c r="E17" t="s">
-        <v>194</v>
+        <v>89</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1689,6 +1948,188 @@
         <v>0</v>
       </c>
       <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="6">
+        <v>3</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+      <c r="D19" s="6">
+        <v>5</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="6">
+        <v>19</v>
+      </c>
+      <c r="C21" s="6">
+        <v>31</v>
+      </c>
+      <c r="D21" s="6">
+        <v>244</v>
+      </c>
+      <c r="E21" s="6">
+        <v>15</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="6">
+        <v>8</v>
+      </c>
+      <c r="C22" s="6">
+        <v>5</v>
+      </c>
+      <c r="D22" s="6">
+        <v>10</v>
+      </c>
+      <c r="E22" s="6">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B24" t="s">
+        <v>285</v>
+      </c>
+      <c r="C24" t="s">
+        <v>283</v>
+      </c>
+      <c r="D24" t="s">
+        <v>284</v>
+      </c>
+      <c r="E24" t="s">
+        <v>282</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <v>1</v>
       </c>
     </row>
@@ -1700,10 +2141,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76785A13-83EB-4155-886C-9E5565477D2B}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,45 +2161,45 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>201</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1772,19 +2213,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1798,19 +2239,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1824,19 +2265,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>130</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1850,19 +2291,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1876,19 +2317,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>139</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>141</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1902,19 +2343,19 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>146</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1928,19 +2369,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1954,19 +2395,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="E10" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1980,19 +2421,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -2006,19 +2447,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C12" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D12" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -2032,19 +2473,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C13" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E13" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -2058,19 +2499,19 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B14" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C14" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D14" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E14" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -2084,27 +2525,261 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" t="s">
+        <v>180</v>
+      </c>
+      <c r="E15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" t="s">
+        <v>189</v>
+      </c>
+      <c r="D17" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17" t="s">
+        <v>191</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" t="s">
+        <v>193</v>
+      </c>
+      <c r="D18" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" t="s">
         <v>195</v>
       </c>
-      <c r="B15" t="s">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>196</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B19" t="s">
         <v>197</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C19" t="s">
         <v>198</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D19" t="s">
         <v>199</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
+      <c r="E19" t="s">
+        <v>200</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B20" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" t="s">
+        <v>203</v>
+      </c>
+      <c r="D20" t="s">
+        <v>204</v>
+      </c>
+      <c r="E20" t="s">
+        <v>205</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>206</v>
+      </c>
+      <c r="B21" s="6">
+        <v>5</v>
+      </c>
+      <c r="C21" s="6">
+        <v>7</v>
+      </c>
+      <c r="D21" s="6">
+        <v>3</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" s="6">
+        <v>80</v>
+      </c>
+      <c r="C22" s="6">
+        <v>90</v>
+      </c>
+      <c r="D22" s="6">
+        <v>85</v>
+      </c>
+      <c r="E22" s="6">
+        <v>75</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B23" s="6">
+        <v>8</v>
+      </c>
+      <c r="C23" s="6">
+        <v>9</v>
+      </c>
+      <c r="D23" s="6">
+        <v>2</v>
+      </c>
+      <c r="E23" s="6">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B24" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <v>2</v>
       </c>
     </row>
@@ -2115,16 +2790,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33252635-A11D-41C3-8881-606A1B9AA576}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="96.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="4" max="4" width="25.140625" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
@@ -2135,45 +2810,45 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>201</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>211</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>212</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>213</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>214</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -2187,19 +2862,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>215</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>219</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2213,19 +2888,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>220</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>221</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>222</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>223</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>224</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -2239,19 +2914,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>225</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>226</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>227</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>228</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>229</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -2265,19 +2940,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>230</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>231</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>232</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>233</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>234</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2291,19 +2966,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>236</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>237</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>238</v>
       </c>
       <c r="E7" t="s">
-        <v>100</v>
+        <v>239</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2317,19 +2992,19 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>241</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>242</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>243</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>244</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -2343,19 +3018,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>245</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>246</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>247</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>248</v>
       </c>
       <c r="E9" t="s">
-        <v>109</v>
+        <v>249</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -2369,19 +3044,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>250</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="E10" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -2390,6 +3065,188 @@
         <v>0</v>
       </c>
       <c r="H10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C11" t="s">
+        <v>253</v>
+      </c>
+      <c r="D11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E11" t="s">
+        <v>255</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" t="s">
+        <v>259</v>
+      </c>
+      <c r="E12" t="s">
+        <v>260</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B13" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D13" t="s">
+        <v>264</v>
+      </c>
+      <c r="E13" t="s">
+        <v>265</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>266</v>
+      </c>
+      <c r="B14" t="s">
+        <v>267</v>
+      </c>
+      <c r="C14" t="s">
+        <v>268</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="E14" t="s">
+        <v>270</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1953</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1937</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1985</v>
+      </c>
+      <c r="E15" s="6">
+        <v>2001</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>272</v>
+      </c>
+      <c r="B16" t="s">
+        <v>273</v>
+      </c>
+      <c r="C16" t="s">
+        <v>274</v>
+      </c>
+      <c r="D16" t="s">
+        <v>275</v>
+      </c>
+      <c r="E16" t="s">
+        <v>276</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>277</v>
+      </c>
+      <c r="B17" t="s">
+        <v>278</v>
+      </c>
+      <c r="C17" t="s">
+        <v>279</v>
+      </c>
+      <c r="D17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" t="s">
+        <v>280</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>3</v>
       </c>
     </row>
@@ -2408,6 +3265,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="870dce62-94b7-4185-9b0a-7139e4ecfd19">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d36953de-bf6f-4d09-a956-94a114c2afc4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A5508CC596D91468A4B201947B3B280" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14a927ece4f3ea2a91f30cf304bc7235">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="870dce62-94b7-4185-9b0a-7139e4ecfd19" xmlns:ns3="d36953de-bf6f-4d09-a956-94a114c2afc4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d7e2e7fca528be30e87c80d0fbe5901d" ns2:_="" ns3:_="">
     <xsd:import namespace="870dce62-94b7-4185-9b0a-7139e4ecfd19"/>
@@ -2602,17 +3470,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="870dce62-94b7-4185-9b0a-7139e4ecfd19">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d36953de-bf6f-4d09-a956-94a114c2afc4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D4AF99-232C-48F0-A5C9-BB1B5A9492D9}">
   <ds:schemaRefs>
@@ -2622,6 +3479,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA73119-806C-48D3-8981-20146BD94452}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="870dce62-94b7-4185-9b0a-7139e4ecfd19"/>
+    <ds:schemaRef ds:uri="d36953de-bf6f-4d09-a956-94a114c2afc4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E8E05AB-1B47-4C51-8E09-465A5CFFA283}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2638,21 +3506,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CA73119-806C-48D3-8981-20146BD94452}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d36953de-bf6f-4d09-a956-94a114c2afc4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="870dce62-94b7-4185-9b0a-7139e4ecfd19"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>